<commit_message>
- Added String subsitute features. - Added wrapStrings boolean to parent config - Added wrapStringChar to parent config - Added wrapStrings boolean to sheet config - Added wrapStringChar to sheet config - Added parent config format in the settings.json     - sourceFile and outputPath can now be specified by settings     - source and outputPath are overriden when pressent as commandline       arguments.
</commit_message>
<xml_diff>
--- a/examples/test.xlsx
+++ b/examples/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="49">
   <si>
     <t xml:space="preserve">Sheet 2</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t xml:space="preserve">foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test123”</t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1788,10 +1791,10 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1880,7 +1883,7 @@
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>47</v>

</xml_diff>